<commit_message>
finish working tests in one_reaction_linear.xlsx
</commit_message>
<xml_diff>
--- a/tests/fixtures/dynamic_tests/one_reaction_linear.xlsx
+++ b/tests/fixtures/dynamic_tests/one_reaction_linear.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-34220" yWindow="5560" windowWidth="32800" windowHeight="15540" tabRatio="500" firstSheet="9" activeTab="19"/>
+    <workbookView xWindow="-21500" yWindow="8340" windowWidth="21480" windowHeight="13260" tabRatio="500" activeTab="1"/>
     <workbookView xWindow="1620" yWindow="4080" windowWidth="35880" windowHeight="16800" tabRatio="500" activeTab="10"/>
   </bookViews>
   <sheets>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="235">
   <si>
     <t>!!!ObjTables ObjTablesVersion='0.0.8'</t>
   </si>
@@ -776,9 +776,6 @@
     <t>Linear</t>
   </si>
   <si>
-    <t>Linear until reactant depleted</t>
-  </si>
-  <si>
     <t>!Pop_A_c_</t>
   </si>
   <si>
@@ -789,6 +786,12 @@
   </si>
   <si>
     <t>Computation for Pop_B_c_</t>
+  </si>
+  <si>
+    <t>Linear populations, static aggregates</t>
+  </si>
+  <si>
+    <t>See formulas in Computation columns</t>
   </si>
 </sst>
 </file>
@@ -963,7 +966,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1078,9 +1081,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1792,16 +1792,16 @@
         <v>199</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>232</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>233</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>219</v>
@@ -2008,13 +2008,14 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="10" max="18" width="16" customWidth="1"/>
+    <col min="10" max="17" width="16" customWidth="1"/>
+    <col min="18" max="18" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2033,59 +2034,59 @@
       <c r="K1" s="39"/>
       <c r="L1" s="39"/>
     </row>
-    <row r="2" spans="1:18" s="42" customFormat="1" ht="65" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
+    <row r="2" spans="1:18" s="41" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+      <c r="A2" s="40" t="s">
         <v>199</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="40" t="s">
         <v>200</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="40" t="s">
         <v>201</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="40" t="s">
         <v>202</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="40" t="s">
         <v>221</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="40" t="s">
         <v>222</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="40" t="s">
         <v>223</v>
       </c>
-      <c r="J2" s="41" t="s">
+      <c r="J2" s="40" t="s">
         <v>204</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="40" t="s">
         <v>205</v>
       </c>
-      <c r="L2" s="41" t="s">
+      <c r="L2" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="M2" s="41" t="s">
+      <c r="M2" s="40" t="s">
         <v>207</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="N2" s="40" t="s">
         <v>224</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="O2" s="40" t="s">
         <v>225</v>
       </c>
-      <c r="P2" s="41" t="s">
+      <c r="P2" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="Q2" s="41" t="s">
+      <c r="Q2" s="40" t="s">
         <v>227</v>
       </c>
-      <c r="R2" s="41" t="s">
+      <c r="R2" s="40" t="s">
         <v>219</v>
       </c>
     </row>
@@ -2093,11 +2094,25 @@
       <c r="A3">
         <v>0</v>
       </c>
+      <c r="J3">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K3">
+        <v>9.9999999999999991E-22</v>
+      </c>
       <c r="L3">
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="M3">
         <v>3.019161891685753E-22</v>
+      </c>
+      <c r="N3">
+        <f>density_c * volume_c</f>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O3">
+        <f>volume_c</f>
+        <v>9.9999999999999991E-22</v>
       </c>
       <c r="P3">
         <f>(Molecular_weight_A* '!!Species trajectories'!D3 + Molecular_weight_B * '!!Species trajectories'!E3)/avogadros_constant</f>
@@ -2107,16 +2122,33 @@
         <f>P3/density_c</f>
         <v>3.019161891685753E-22</v>
       </c>
+      <c r="R3" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>100</v>
       </c>
+      <c r="J4">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K4">
+        <v>9.9999999999999991E-22</v>
+      </c>
       <c r="L4">
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="M4">
         <v>3.019161891685753E-22</v>
+      </c>
+      <c r="N4">
+        <f>density_c * volume_c</f>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O4">
+        <f>volume_c</f>
+        <v>9.9999999999999991E-22</v>
       </c>
       <c r="P4">
         <f>(Molecular_weight_A* '!!Species trajectories'!D4 + Molecular_weight_B * '!!Species trajectories'!E4)/avogadros_constant</f>
@@ -2131,11 +2163,25 @@
       <c r="A5">
         <v>200</v>
       </c>
+      <c r="J5">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K5">
+        <v>9.9999999999999991E-22</v>
+      </c>
       <c r="L5">
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="M5">
         <v>3.019161891685753E-22</v>
+      </c>
+      <c r="N5">
+        <f>density_c * volume_c</f>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O5">
+        <f>volume_c</f>
+        <v>9.9999999999999991E-22</v>
       </c>
       <c r="P5">
         <f>(Molecular_weight_A* '!!Species trajectories'!D5 + Molecular_weight_B * '!!Species trajectories'!E5)/avogadros_constant</f>
@@ -2150,11 +2196,25 @@
       <c r="A6">
         <v>300</v>
       </c>
+      <c r="J6">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K6">
+        <v>9.9999999999999991E-22</v>
+      </c>
       <c r="L6">
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="M6">
         <v>3.019161891685753E-22</v>
+      </c>
+      <c r="N6">
+        <f>density_c * volume_c</f>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O6">
+        <f>volume_c</f>
+        <v>9.9999999999999991E-22</v>
       </c>
       <c r="P6">
         <f>(Molecular_weight_A* '!!Species trajectories'!D6 + Molecular_weight_B * '!!Species trajectories'!E6)/avogadros_constant</f>
@@ -2169,11 +2229,25 @@
       <c r="A7">
         <v>400</v>
       </c>
+      <c r="J7">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K7">
+        <v>9.9999999999999991E-22</v>
+      </c>
       <c r="L7">
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="M7">
         <v>3.019161891685753E-22</v>
+      </c>
+      <c r="N7">
+        <f>density_c * volume_c</f>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O7">
+        <f>volume_c</f>
+        <v>9.9999999999999991E-22</v>
       </c>
       <c r="P7">
         <f>(Molecular_weight_A* '!!Species trajectories'!D7 + Molecular_weight_B * '!!Species trajectories'!E7)/avogadros_constant</f>
@@ -2188,11 +2262,25 @@
       <c r="A8">
         <v>500</v>
       </c>
+      <c r="J8">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K8">
+        <v>9.9999999999999991E-22</v>
+      </c>
       <c r="L8">
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="M8">
         <v>3.019161891685753E-22</v>
+      </c>
+      <c r="N8">
+        <f>density_c * volume_c</f>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O8">
+        <f>volume_c</f>
+        <v>9.9999999999999991E-22</v>
       </c>
       <c r="P8">
         <f>(Molecular_weight_A* '!!Species trajectories'!D8 + Molecular_weight_B * '!!Species trajectories'!E8)/avogadros_constant</f>
@@ -2207,13 +2295,26 @@
       <c r="A9">
         <v>600</v>
       </c>
+      <c r="J9">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K9">
+        <v>9.9999999999999991E-22</v>
+      </c>
       <c r="L9">
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="M9">
         <v>3.019161891685753E-22</v>
       </c>
-      <c r="N9" s="40"/>
+      <c r="N9">
+        <f>density_c * volume_c</f>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O9">
+        <f>volume_c</f>
+        <v>9.9999999999999991E-22</v>
+      </c>
       <c r="P9">
         <f>(Molecular_weight_A* '!!Species trajectories'!D9 + Molecular_weight_B * '!!Species trajectories'!E9)/avogadros_constant</f>
         <v>3.3210780808543282E-19</v>
@@ -2227,11 +2328,25 @@
       <c r="A10">
         <v>700</v>
       </c>
+      <c r="J10">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K10">
+        <v>9.9999999999999991E-22</v>
+      </c>
       <c r="L10">
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="M10">
         <v>3.019161891685753E-22</v>
+      </c>
+      <c r="N10">
+        <f>density_c * volume_c</f>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O10">
+        <f>volume_c</f>
+        <v>9.9999999999999991E-22</v>
       </c>
       <c r="P10">
         <f>(Molecular_weight_A* '!!Species trajectories'!D10 + Molecular_weight_B * '!!Species trajectories'!E10)/avogadros_constant</f>
@@ -2246,11 +2361,25 @@
       <c r="A11">
         <v>800</v>
       </c>
+      <c r="J11">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K11">
+        <v>9.9999999999999991E-22</v>
+      </c>
       <c r="L11">
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="M11">
         <v>3.019161891685753E-22</v>
+      </c>
+      <c r="N11">
+        <f>density_c * volume_c</f>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O11">
+        <f>volume_c</f>
+        <v>9.9999999999999991E-22</v>
       </c>
       <c r="P11">
         <f>(Molecular_weight_A* '!!Species trajectories'!D11 + Molecular_weight_B * '!!Species trajectories'!E11)/avogadros_constant</f>
@@ -2265,11 +2394,25 @@
       <c r="A12">
         <v>900</v>
       </c>
+      <c r="J12">
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="K12">
+        <v>9.9999999999999991E-22</v>
+      </c>
       <c r="L12">
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="M12">
         <v>3.019161891685753E-22</v>
+      </c>
+      <c r="N12">
+        <f>density_c * volume_c</f>
+        <v>1.0999999999999999E-18</v>
+      </c>
+      <c r="O12">
+        <f>volume_c</f>
+        <v>9.9999999999999991E-22</v>
       </c>
       <c r="P12">
         <f>(Molecular_weight_A* '!!Species trajectories'!D12 + Molecular_weight_B * '!!Species trajectories'!E12)/avogadros_constant</f>
@@ -2298,20 +2441,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:5" s="41" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A1" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="48" t="s">
         <v>218</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="49" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="48" t="s">
         <v>215</v>
       </c>
     </row>
@@ -2544,11 +2687,11 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -3587,28 +3730,28 @@
       <c r="F3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="M3" s="43" t="s">
+      <c r="M3" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="43" t="s">
+      <c r="N3" s="42" t="s">
         <v>51</v>
       </c>
       <c r="O3" s="6"/>
@@ -4954,8 +5097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
   </sheetViews>
@@ -4986,7 +5129,7 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -5072,7 +5215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
@@ -5090,7 +5233,7 @@
     <col min="7" max="7" width="11.83203125" style="16" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="16" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" style="16" customWidth="1"/>
-    <col min="10" max="10" width="13.5" style="44" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="43" customWidth="1"/>
     <col min="11" max="1026" width="8.83203125" style="1" customWidth="1"/>
     <col min="1027" max="1028" width="9" style="1" customWidth="1"/>
     <col min="1029" max="16384" width="9" style="1"/>
@@ -5144,7 +5287,7 @@
       <c r="B3" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="46">
         <v>0.3</v>
       </c>
       <c r="F3" s="16" t="s">
@@ -5170,13 +5313,13 @@
       <c r="A5" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="47">
         <v>6.0221408570000002E+23</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="44" t="s">
         <v>208</v>
       </c>
     </row>
@@ -5204,16 +5347,16 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
       <c r="D8">
         <v>100</v>
       </c>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46" t="s">
+      <c r="E8" s="45"/>
+      <c r="F8" s="45" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5304,26 +5447,26 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="H2" s="56"/>
-      <c r="I2" s="58" t="s">
+      <c r="H2" s="55"/>
+      <c r="I2" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="Q2" s="59" t="s">
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="Q2" s="58" t="s">
         <v>142</v>
       </c>
-      <c r="R2" s="56"/>
-      <c r="S2" s="59" t="s">
+      <c r="R2" s="55"/>
+      <c r="S2" s="58" t="s">
         <v>143</v>
       </c>
-      <c r="T2" s="56"/>
+      <c r="T2" s="55"/>
     </row>
     <row r="3" spans="1:23" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5489,10 +5632,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="H2" s="56"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -6080,19 +6223,19 @@
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
-      <c r="H2" s="51" t="s">
+      <c r="H2" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
       <c r="L2" s="31"/>
-      <c r="M2" s="54" t="s">
+      <c r="M2" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
@@ -8278,14 +8421,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">

</xml_diff>

<commit_message>
analysis of new internal ODE step data
</commit_message>
<xml_diff>
--- a/tests/fixtures/dynamic_tests/one_reaction_linear.xlsx
+++ b/tests/fixtures/dynamic_tests/one_reaction_linear.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-21500" yWindow="8340" windowWidth="21480" windowHeight="13260" tabRatio="500" activeTab="1"/>
-    <workbookView xWindow="1620" yWindow="4080" windowWidth="35880" windowHeight="16800" tabRatio="500" activeTab="10"/>
+    <workbookView xWindow="-21500" yWindow="8340" windowWidth="21480" windowHeight="13260" tabRatio="500" firstSheet="9" activeTab="9"/>
+    <workbookView xWindow="1620" yWindow="4080" windowWidth="35880" windowHeight="16800" tabRatio="500" firstSheet="7" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -1755,12 +1755,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A3:A12"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1818,11 +1818,11 @@
         <v>100</v>
       </c>
       <c r="D3">
-        <f>initial_pop_a - k_cat_1_for*$A3</f>
+        <f>MAX(0, initial_pop_a - k_cat_1_for*$A3)</f>
         <v>900</v>
       </c>
       <c r="E3">
-        <f>initial_pop_b + k_cat_1_for * A3</f>
+        <f>initial_pop_b + initial_pop_a - D3</f>
         <v>100</v>
       </c>
     </row>
@@ -1837,11 +1837,11 @@
         <v>200</v>
       </c>
       <c r="D4">
-        <f>initial_pop_a - k_cat_1_for*$A4</f>
+        <f>MAX(0, initial_pop_a - k_cat_1_for*$A4)</f>
         <v>800</v>
       </c>
       <c r="E4">
-        <f>initial_pop_b + k_cat_1_for * A4</f>
+        <f>initial_pop_b + initial_pop_a - D4</f>
         <v>200</v>
       </c>
     </row>
@@ -1856,11 +1856,11 @@
         <v>300</v>
       </c>
       <c r="D5">
-        <f>initial_pop_a - k_cat_1_for*$A5</f>
+        <f>MAX(0, initial_pop_a - k_cat_1_for*$A5)</f>
         <v>700</v>
       </c>
       <c r="E5">
-        <f>initial_pop_b + k_cat_1_for * A5</f>
+        <f>initial_pop_b + initial_pop_a - D5</f>
         <v>300</v>
       </c>
     </row>
@@ -1875,11 +1875,11 @@
         <v>400</v>
       </c>
       <c r="D6">
-        <f>initial_pop_a - k_cat_1_for*$A6</f>
+        <f>MAX(0, initial_pop_a - k_cat_1_for*$A6)</f>
         <v>600</v>
       </c>
       <c r="E6">
-        <f>initial_pop_b + k_cat_1_for * A6</f>
+        <f>initial_pop_b + initial_pop_a - D6</f>
         <v>400</v>
       </c>
     </row>
@@ -1894,11 +1894,11 @@
         <v>500</v>
       </c>
       <c r="D7">
-        <f>initial_pop_a - k_cat_1_for*$A7</f>
+        <f>MAX(0, initial_pop_a - k_cat_1_for*$A7)</f>
         <v>500</v>
       </c>
       <c r="E7">
-        <f>initial_pop_b + k_cat_1_for * A7</f>
+        <f>initial_pop_b + initial_pop_a - D7</f>
         <v>500</v>
       </c>
     </row>
@@ -1913,11 +1913,11 @@
         <v>600</v>
       </c>
       <c r="D8">
-        <f>initial_pop_a - k_cat_1_for*$A8</f>
+        <f>MAX(0, initial_pop_a - k_cat_1_for*$A8)</f>
         <v>400</v>
       </c>
       <c r="E8">
-        <f>initial_pop_b + k_cat_1_for * A8</f>
+        <f>initial_pop_b + initial_pop_a - D8</f>
         <v>600</v>
       </c>
     </row>
@@ -1932,11 +1932,11 @@
         <v>700</v>
       </c>
       <c r="D9">
-        <f>initial_pop_a - k_cat_1_for*$A9</f>
+        <f>MAX(0, initial_pop_a - k_cat_1_for*$A9)</f>
         <v>300</v>
       </c>
       <c r="E9">
-        <f>initial_pop_b + k_cat_1_for * A9</f>
+        <f>initial_pop_b + initial_pop_a - D9</f>
         <v>700</v>
       </c>
     </row>
@@ -1951,11 +1951,11 @@
         <v>800</v>
       </c>
       <c r="D10">
-        <f>initial_pop_a - k_cat_1_for*$A10</f>
+        <f>MAX(0, initial_pop_a - k_cat_1_for*$A10)</f>
         <v>200</v>
       </c>
       <c r="E10">
-        <f>initial_pop_b + k_cat_1_for * A10</f>
+        <f>initial_pop_b + initial_pop_a - D10</f>
         <v>800</v>
       </c>
     </row>
@@ -1970,11 +1970,11 @@
         <v>900</v>
       </c>
       <c r="D11">
-        <f>initial_pop_a - k_cat_1_for*$A11</f>
+        <f>MAX(0, initial_pop_a - k_cat_1_for*$A11)</f>
         <v>100</v>
       </c>
       <c r="E11">
-        <f>initial_pop_b + k_cat_1_for * A11</f>
+        <f>initial_pop_b + initial_pop_a - D11</f>
         <v>900</v>
       </c>
     </row>
@@ -1989,11 +1989,11 @@
         <v>1000</v>
       </c>
       <c r="D12">
-        <f>initial_pop_a - k_cat_1_for*$A12</f>
+        <f>MAX(0, initial_pop_a - k_cat_1_for*$A12)</f>
         <v>0</v>
       </c>
       <c r="E12">
-        <f>initial_pop_b + k_cat_1_for * A12</f>
+        <f>initial_pop_b + initial_pop_a - D12</f>
         <v>1000</v>
       </c>
     </row>
@@ -2007,7 +2007,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
       <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
@@ -2107,11 +2107,11 @@
         <v>3.019161891685753E-22</v>
       </c>
       <c r="N3">
-        <f>density_c * volume_c</f>
+        <f t="shared" ref="N3:N12" si="0">density_c * volume_c</f>
         <v>1.0999999999999999E-18</v>
       </c>
       <c r="O3">
-        <f>volume_c</f>
+        <f t="shared" ref="O3:O12" si="1">volume_c</f>
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="P3">
@@ -2119,7 +2119,7 @@
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="Q3">
-        <f>P3/density_c</f>
+        <f t="shared" ref="Q3:Q12" si="2">P3/density_c</f>
         <v>3.019161891685753E-22</v>
       </c>
       <c r="R3" t="s">
@@ -2143,11 +2143,11 @@
         <v>3.019161891685753E-22</v>
       </c>
       <c r="N4">
-        <f>density_c * volume_c</f>
+        <f t="shared" si="0"/>
         <v>1.0999999999999999E-18</v>
       </c>
       <c r="O4">
-        <f>volume_c</f>
+        <f t="shared" si="1"/>
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="P4">
@@ -2155,7 +2155,7 @@
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="Q4">
-        <f>P4/density_c</f>
+        <f t="shared" si="2"/>
         <v>3.019161891685753E-22</v>
       </c>
     </row>
@@ -2176,11 +2176,11 @@
         <v>3.019161891685753E-22</v>
       </c>
       <c r="N5">
-        <f>density_c * volume_c</f>
+        <f t="shared" si="0"/>
         <v>1.0999999999999999E-18</v>
       </c>
       <c r="O5">
-        <f>volume_c</f>
+        <f t="shared" si="1"/>
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="P5">
@@ -2188,7 +2188,7 @@
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="Q5">
-        <f>P5/density_c</f>
+        <f t="shared" si="2"/>
         <v>3.019161891685753E-22</v>
       </c>
     </row>
@@ -2209,11 +2209,11 @@
         <v>3.019161891685753E-22</v>
       </c>
       <c r="N6">
-        <f>density_c * volume_c</f>
+        <f t="shared" si="0"/>
         <v>1.0999999999999999E-18</v>
       </c>
       <c r="O6">
-        <f>volume_c</f>
+        <f t="shared" si="1"/>
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="P6">
@@ -2221,7 +2221,7 @@
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="Q6">
-        <f>P6/density_c</f>
+        <f t="shared" si="2"/>
         <v>3.019161891685753E-22</v>
       </c>
     </row>
@@ -2242,11 +2242,11 @@
         <v>3.019161891685753E-22</v>
       </c>
       <c r="N7">
-        <f>density_c * volume_c</f>
+        <f t="shared" si="0"/>
         <v>1.0999999999999999E-18</v>
       </c>
       <c r="O7">
-        <f>volume_c</f>
+        <f t="shared" si="1"/>
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="P7">
@@ -2254,7 +2254,7 @@
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="Q7">
-        <f>P7/density_c</f>
+        <f t="shared" si="2"/>
         <v>3.019161891685753E-22</v>
       </c>
     </row>
@@ -2275,11 +2275,11 @@
         <v>3.019161891685753E-22</v>
       </c>
       <c r="N8">
-        <f>density_c * volume_c</f>
+        <f t="shared" si="0"/>
         <v>1.0999999999999999E-18</v>
       </c>
       <c r="O8">
-        <f>volume_c</f>
+        <f t="shared" si="1"/>
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="P8">
@@ -2287,7 +2287,7 @@
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="Q8">
-        <f>P8/density_c</f>
+        <f t="shared" si="2"/>
         <v>3.019161891685753E-22</v>
       </c>
     </row>
@@ -2308,11 +2308,11 @@
         <v>3.019161891685753E-22</v>
       </c>
       <c r="N9">
-        <f>density_c * volume_c</f>
+        <f t="shared" si="0"/>
         <v>1.0999999999999999E-18</v>
       </c>
       <c r="O9">
-        <f>volume_c</f>
+        <f t="shared" si="1"/>
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="P9">
@@ -2320,7 +2320,7 @@
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="Q9">
-        <f>P9/density_c</f>
+        <f t="shared" si="2"/>
         <v>3.019161891685753E-22</v>
       </c>
     </row>
@@ -2341,11 +2341,11 @@
         <v>3.019161891685753E-22</v>
       </c>
       <c r="N10">
-        <f>density_c * volume_c</f>
+        <f t="shared" si="0"/>
         <v>1.0999999999999999E-18</v>
       </c>
       <c r="O10">
-        <f>volume_c</f>
+        <f t="shared" si="1"/>
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="P10">
@@ -2353,7 +2353,7 @@
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="Q10">
-        <f>P10/density_c</f>
+        <f t="shared" si="2"/>
         <v>3.019161891685753E-22</v>
       </c>
     </row>
@@ -2374,11 +2374,11 @@
         <v>3.019161891685753E-22</v>
       </c>
       <c r="N11">
-        <f>density_c * volume_c</f>
+        <f t="shared" si="0"/>
         <v>1.0999999999999999E-18</v>
       </c>
       <c r="O11">
-        <f>volume_c</f>
+        <f t="shared" si="1"/>
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="P11">
@@ -2386,7 +2386,7 @@
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="Q11">
-        <f>P11/density_c</f>
+        <f t="shared" si="2"/>
         <v>3.019161891685753E-22</v>
       </c>
     </row>
@@ -2407,11 +2407,11 @@
         <v>3.019161891685753E-22</v>
       </c>
       <c r="N12">
-        <f>density_c * volume_c</f>
+        <f t="shared" si="0"/>
         <v>1.0999999999999999E-18</v>
       </c>
       <c r="O12">
-        <f>volume_c</f>
+        <f t="shared" si="1"/>
         <v>9.9999999999999991E-22</v>
       </c>
       <c r="P12">
@@ -2419,7 +2419,7 @@
         <v>3.3210780808543282E-19</v>
       </c>
       <c r="Q12">
-        <f>P12/density_c</f>
+        <f t="shared" si="2"/>
         <v>3.019161891685753E-22</v>
       </c>
     </row>
@@ -2650,7 +2650,7 @@
   <dimension ref="A1:AMM5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -5097,7 +5097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
@@ -5218,8 +5218,8 @@
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
enable optional change of compartment volumes; add doc strings
</commit_message>
<xml_diff>
--- a/tests/fixtures/dynamic_tests/one_reaction_linear.xlsx
+++ b/tests/fixtures/dynamic_tests/one_reaction_linear.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-21500" yWindow="8340" windowWidth="21480" windowHeight="13260" tabRatio="500" firstSheet="9" activeTab="9"/>
-    <workbookView xWindow="1620" yWindow="4080" windowWidth="35880" windowHeight="16800" tabRatio="500" firstSheet="7" activeTab="19"/>
+    <workbookView xWindow="1620" yWindow="4080" windowWidth="35880" windowHeight="16800" tabRatio="500" firstSheet="7" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -1818,11 +1818,11 @@
         <v>100</v>
       </c>
       <c r="D3">
-        <f>MAX(0, initial_pop_a - k_cat_1_for*$A3)</f>
+        <f t="shared" ref="D3:D12" si="0">MAX(0, initial_pop_a - k_cat_1_for*$A3)</f>
         <v>900</v>
       </c>
       <c r="E3">
-        <f>initial_pop_b + initial_pop_a - D3</f>
+        <f t="shared" ref="E3:E12" si="1">initial_pop_b + initial_pop_a - D3</f>
         <v>100</v>
       </c>
     </row>
@@ -1837,11 +1837,11 @@
         <v>200</v>
       </c>
       <c r="D4">
-        <f>MAX(0, initial_pop_a - k_cat_1_for*$A4)</f>
+        <f t="shared" si="0"/>
         <v>800</v>
       </c>
       <c r="E4">
-        <f>initial_pop_b + initial_pop_a - D4</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
     </row>
@@ -1856,11 +1856,11 @@
         <v>300</v>
       </c>
       <c r="D5">
-        <f>MAX(0, initial_pop_a - k_cat_1_for*$A5)</f>
+        <f t="shared" si="0"/>
         <v>700</v>
       </c>
       <c r="E5">
-        <f>initial_pop_b + initial_pop_a - D5</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
     </row>
@@ -1875,11 +1875,11 @@
         <v>400</v>
       </c>
       <c r="D6">
-        <f>MAX(0, initial_pop_a - k_cat_1_for*$A6)</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="E6">
-        <f>initial_pop_b + initial_pop_a - D6</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
     </row>
@@ -1894,11 +1894,11 @@
         <v>500</v>
       </c>
       <c r="D7">
-        <f>MAX(0, initial_pop_a - k_cat_1_for*$A7)</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="E7">
-        <f>initial_pop_b + initial_pop_a - D7</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
     </row>
@@ -1913,11 +1913,11 @@
         <v>600</v>
       </c>
       <c r="D8">
-        <f>MAX(0, initial_pop_a - k_cat_1_for*$A8)</f>
+        <f t="shared" si="0"/>
         <v>400</v>
       </c>
       <c r="E8">
-        <f>initial_pop_b + initial_pop_a - D8</f>
+        <f t="shared" si="1"/>
         <v>600</v>
       </c>
     </row>
@@ -1932,11 +1932,11 @@
         <v>700</v>
       </c>
       <c r="D9">
-        <f>MAX(0, initial_pop_a - k_cat_1_for*$A9)</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="E9">
-        <f>initial_pop_b + initial_pop_a - D9</f>
+        <f t="shared" si="1"/>
         <v>700</v>
       </c>
     </row>
@@ -1951,11 +1951,11 @@
         <v>800</v>
       </c>
       <c r="D10">
-        <f>MAX(0, initial_pop_a - k_cat_1_for*$A10)</f>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="E10">
-        <f>initial_pop_b + initial_pop_a - D10</f>
+        <f t="shared" si="1"/>
         <v>800</v>
       </c>
     </row>
@@ -1970,11 +1970,11 @@
         <v>900</v>
       </c>
       <c r="D11">
-        <f>MAX(0, initial_pop_a - k_cat_1_for*$A11)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="E11">
-        <f>initial_pop_b + initial_pop_a - D11</f>
+        <f t="shared" si="1"/>
         <v>900</v>
       </c>
     </row>
@@ -1989,11 +1989,11 @@
         <v>1000</v>
       </c>
       <c r="D12">
-        <f>MAX(0, initial_pop_a - k_cat_1_for*$A12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E12">
-        <f>initial_pop_b + initial_pop_a - D12</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
     </row>
@@ -2652,15 +2652,17 @@
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18" style="16" customWidth="1"/>
-    <col min="2" max="2" width="19" style="16" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="50.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="19" style="16" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="16" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" style="16" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.1640625" style="16" customWidth="1"/>
@@ -4812,11 +4814,14 @@
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="23.6640625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="16" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" style="16" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" style="16" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" style="16" customWidth="1"/>
@@ -4903,12 +4908,15 @@
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" style="16" customWidth="1"/>
-    <col min="2" max="3" width="9" style="16" customWidth="1"/>
+    <col min="2" max="2" width="9" style="16" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="16" customWidth="1"/>
     <col min="4" max="4" width="10.5" style="16" customWidth="1"/>
     <col min="5" max="6" width="9" style="16" customWidth="1"/>
     <col min="7" max="16384" width="9" style="16"/>
@@ -4969,12 +4977,14 @@
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="4" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="4" customWidth="1"/>
     <col min="4" max="5" width="8.83203125" style="4" customWidth="1"/>
     <col min="6" max="1026" width="8.83203125" style="16" customWidth="1"/>
@@ -5032,12 +5042,14 @@
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD5"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15" style="4" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="11" style="4" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" style="4" customWidth="1"/>
@@ -5218,14 +5230,14 @@
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="31.1640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" style="16" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" style="16" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="16" customWidth="1"/>
     <col min="5" max="5" width="8.1640625" style="16" customWidth="1"/>

</xml_diff>